<commit_message>
My Latest updated version
</commit_message>
<xml_diff>
--- a/src/test/java/com/testData/Jombone_SignUpFirstNameData.xlsx
+++ b/src/test/java/com/testData/Jombone_SignUpFirstNameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aila\eclipse-workspace\jombone\src\test\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70885E60-CD69-4558-8C66-B556BCD249F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E27C90-E0F7-4743-A25D-594235346388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{F2CA8C7A-6456-4EFF-93E9-06EFD680AA06}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>FirstName</t>
   </si>
@@ -58,34 +58,37 @@
     <t>Saritha123</t>
   </si>
   <si>
-    <t>abcdefghijklmnopqrstuvwxyzabcdefghijklmnopqrstuvwxyz</t>
-  </si>
-  <si>
-    <t>arithlakkLLK1@gmail.com</t>
-  </si>
-  <si>
-    <t>416-858-7777</t>
-  </si>
-  <si>
     <t>Bhargavi2022$</t>
   </si>
   <si>
-    <t>arithlakkLLK2@gmail.com</t>
-  </si>
-  <si>
-    <t>arithlakkLLK14@gmail.com</t>
-  </si>
-  <si>
-    <t>arithlakkLLK51@gmail.com</t>
-  </si>
-  <si>
-    <t>arithlakkLLK81@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>mobile</t>
+  </si>
+  <si>
+    <t>Sarita1@gmail.com</t>
+  </si>
+  <si>
+    <t>Sarita2@gmail.com</t>
+  </si>
+  <si>
+    <t>Sarita3@gmail.com</t>
+  </si>
+  <si>
+    <t>Sarita4@gmail.com</t>
+  </si>
+  <si>
+    <t>416-858-7771</t>
+  </si>
+  <si>
+    <t>416-858-7772</t>
+  </si>
+  <si>
+    <t>416-858-7773</t>
+  </si>
+  <si>
+    <t>416-858-7774</t>
   </si>
 </sst>
 </file>
@@ -136,11 +139,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -457,18 +457,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47EA19F-2033-421A-BDD3-234B86A26070}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -491,19 +491,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,14 +513,14 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,14 +530,14 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -547,42 +547,26 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{83BD06F1-D1DE-4390-BE92-06D4CC64F122}"/>
-    <hyperlink ref="C3:C6" r:id="rId2" display="arithlakkLLK1@gmail.com" xr:uid="{B1458576-090F-4EAD-88AB-C2614EB52EC3}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{40519F28-70CF-4365-B4DC-F9D9FB93CDE0}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{6F1F83A7-73A3-4011-BEF5-0EAF2E119521}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{AB368B7F-2350-4583-A770-73520D5C3791}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{4AE5E155-906E-45AB-8596-C4AFB6C4EDC6}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="Sarita1@gmail.com" xr:uid="{C1A3A0DE-1846-438D-9B6D-17E0EABCCCBC}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{C04AC83B-B53B-4857-88A8-72F33822479D}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{9A5BB50B-83AE-47B7-B63B-0500EFB38B10}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{B6F97B6C-9E4F-4156-896F-26F9A405BC6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>